<commit_message>
Added industry selection to account schema and signup process
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA314C38-11D9-4149-9196-F9B033F44454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B589EF58-73D3-4222-A332-11E6D91D5C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
   <si>
     <t>Week</t>
   </si>
@@ -61,177 +61,6 @@
     <t>Week 8</t>
   </si>
   <si>
-    <t>Jan 20</t>
-  </si>
-  <si>
-    <t>Jan 21</t>
-  </si>
-  <si>
-    <t>Jan 22</t>
-  </si>
-  <si>
-    <t>Jan 23</t>
-  </si>
-  <si>
-    <t>Jan 24</t>
-  </si>
-  <si>
-    <t>Jan 25</t>
-  </si>
-  <si>
-    <t>Jan 26</t>
-  </si>
-  <si>
-    <t>Jan 27</t>
-  </si>
-  <si>
-    <t>Jan 28</t>
-  </si>
-  <si>
-    <t>Jan 29</t>
-  </si>
-  <si>
-    <t>Jan 30</t>
-  </si>
-  <si>
-    <t>Jan 31</t>
-  </si>
-  <si>
-    <t>Feb 1</t>
-  </si>
-  <si>
-    <t>Feb 2</t>
-  </si>
-  <si>
-    <t>Feb 3</t>
-  </si>
-  <si>
-    <t>Feb 4</t>
-  </si>
-  <si>
-    <t>Feb 5</t>
-  </si>
-  <si>
-    <t>Feb 6</t>
-  </si>
-  <si>
-    <t>Feb 7</t>
-  </si>
-  <si>
-    <t>Feb 8</t>
-  </si>
-  <si>
-    <t>Feb 9</t>
-  </si>
-  <si>
-    <t>Feb 10</t>
-  </si>
-  <si>
-    <t>Feb 11</t>
-  </si>
-  <si>
-    <t>Feb 12</t>
-  </si>
-  <si>
-    <t>Feb 13</t>
-  </si>
-  <si>
-    <t>Feb 14</t>
-  </si>
-  <si>
-    <t>Feb 15</t>
-  </si>
-  <si>
-    <t>Feb 16</t>
-  </si>
-  <si>
-    <t>Feb 17</t>
-  </si>
-  <si>
-    <t>Feb 18</t>
-  </si>
-  <si>
-    <t>Feb 19</t>
-  </si>
-  <si>
-    <t>Feb 20</t>
-  </si>
-  <si>
-    <t>Feb 21</t>
-  </si>
-  <si>
-    <t>Feb 22</t>
-  </si>
-  <si>
-    <t>Feb 23</t>
-  </si>
-  <si>
-    <t>Feb 24</t>
-  </si>
-  <si>
-    <t>Feb 25</t>
-  </si>
-  <si>
-    <t>Feb 26</t>
-  </si>
-  <si>
-    <t>Feb 27</t>
-  </si>
-  <si>
-    <t>Feb 28</t>
-  </si>
-  <si>
-    <t>Mar 1</t>
-  </si>
-  <si>
-    <t>Mar 2</t>
-  </si>
-  <si>
-    <t>Mar 3</t>
-  </si>
-  <si>
-    <t>Mar 4</t>
-  </si>
-  <si>
-    <t>Mar 5</t>
-  </si>
-  <si>
-    <t>Mar 6</t>
-  </si>
-  <si>
-    <t>Mar 7</t>
-  </si>
-  <si>
-    <t>Mar 8</t>
-  </si>
-  <si>
-    <t>Mar 9</t>
-  </si>
-  <si>
-    <t>Mar 10</t>
-  </si>
-  <si>
-    <t>Mar 11</t>
-  </si>
-  <si>
-    <t>Mar 12</t>
-  </si>
-  <si>
-    <t>Mar 13</t>
-  </si>
-  <si>
-    <t>Mar 14</t>
-  </si>
-  <si>
-    <t>Mar 15</t>
-  </si>
-  <si>
-    <t>Mar 30</t>
-  </si>
-  <si>
-    <t>Mar 31</t>
-  </si>
-  <si>
     <t>Implement Industry Field</t>
   </si>
   <si>
@@ -403,9 +232,6 @@
     <t>Final Launch &amp; Internal Rollout</t>
   </si>
   <si>
-    <t>Add industry field in company schema</t>
-  </si>
-  <si>
     <t>Allow users to select industry during signup</t>
   </si>
   <si>
@@ -578,6 +404,12 @@
   </si>
   <si>
     <t>Completed Date</t>
+  </si>
+  <si>
+    <t>Add industry field in account schema</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -636,16 +468,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -948,7 +810,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,979 +838,990 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2">
+        <v>45677</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>129</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45677</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2">
+        <v>45678</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>129</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45677</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2">
+        <v>45679</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2">
+        <v>45680</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2">
+        <v>45681</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2">
+        <v>45682</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2">
+        <v>45683</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2">
+        <v>45684</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>77</v>
-      </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2">
+        <v>45685</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
-        <v>78</v>
-      </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2">
+        <v>45686</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2">
+        <v>45687</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2">
+        <v>45688</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2">
+        <v>45689</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>82</v>
-      </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2">
+        <v>45690</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2">
+        <v>45691</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2">
+        <v>45692</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
-        <v>85</v>
-      </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2">
+        <v>45693</v>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
-        <v>86</v>
-      </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2">
+        <v>45694</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>87</v>
-      </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2">
+        <v>45695</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2">
+        <v>45696</v>
+      </c>
+      <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2">
+        <v>45697</v>
+      </c>
+      <c r="C22" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
-        <v>90</v>
-      </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2">
+        <v>45698</v>
+      </c>
+      <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2">
+        <v>45699</v>
+      </c>
+      <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2">
+        <v>45700</v>
+      </c>
+      <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="C25" t="s">
-        <v>93</v>
-      </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2">
+        <v>45701</v>
+      </c>
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
-        <v>94</v>
-      </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2">
+        <v>45702</v>
+      </c>
+      <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
       <c r="D27" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2">
+        <v>45703</v>
+      </c>
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2">
+        <v>45704</v>
+      </c>
+      <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="C29" t="s">
-        <v>97</v>
-      </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2">
+        <v>45705</v>
+      </c>
+      <c r="C30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" t="s">
-        <v>98</v>
-      </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2">
+        <v>45706</v>
+      </c>
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
-        <v>99</v>
-      </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2">
+        <v>45707</v>
+      </c>
+      <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="C32" t="s">
-        <v>100</v>
-      </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2">
+        <v>45708</v>
+      </c>
+      <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" t="s">
-        <v>101</v>
-      </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2">
+        <v>45709</v>
+      </c>
+      <c r="C34" t="s">
         <v>45</v>
       </c>
-      <c r="C34" t="s">
-        <v>102</v>
-      </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2">
+        <v>45710</v>
+      </c>
+      <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="C35" t="s">
-        <v>103</v>
-      </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2">
+        <v>45711</v>
+      </c>
+      <c r="C36" t="s">
         <v>47</v>
       </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
       <c r="D36" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2">
+        <v>45712</v>
+      </c>
+      <c r="C37" t="s">
         <v>48</v>
       </c>
-      <c r="C37" t="s">
-        <v>105</v>
-      </c>
       <c r="D37" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2">
+        <v>45713</v>
+      </c>
+      <c r="C38" t="s">
         <v>49</v>
       </c>
-      <c r="C38" t="s">
-        <v>106</v>
-      </c>
       <c r="D38" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2">
+        <v>45714</v>
+      </c>
+      <c r="C39" t="s">
         <v>50</v>
       </c>
-      <c r="C39" t="s">
-        <v>107</v>
-      </c>
       <c r="D39" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="E39" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2">
+        <v>45715</v>
+      </c>
+      <c r="C40" t="s">
         <v>51</v>
       </c>
-      <c r="C40" t="s">
-        <v>108</v>
-      </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2">
+        <v>45716</v>
+      </c>
+      <c r="C41" t="s">
         <v>52</v>
       </c>
-      <c r="C41" t="s">
-        <v>109</v>
-      </c>
       <c r="D41" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2">
+        <v>45717</v>
+      </c>
+      <c r="C42" t="s">
         <v>53</v>
       </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2">
+        <v>45718</v>
+      </c>
+      <c r="C43" t="s">
         <v>54</v>
       </c>
-      <c r="C43" t="s">
-        <v>111</v>
-      </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2">
+        <v>45719</v>
+      </c>
+      <c r="C44" t="s">
         <v>55</v>
       </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2">
+        <v>45720</v>
+      </c>
+      <c r="C45" t="s">
         <v>56</v>
       </c>
-      <c r="C45" t="s">
-        <v>113</v>
-      </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="E45" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2">
+        <v>45721</v>
+      </c>
+      <c r="C46" t="s">
         <v>57</v>
       </c>
-      <c r="C46" t="s">
-        <v>114</v>
-      </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="E46" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2">
+        <v>45722</v>
+      </c>
+      <c r="C47" t="s">
         <v>58</v>
       </c>
-      <c r="C47" t="s">
-        <v>115</v>
-      </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2">
+        <v>45723</v>
+      </c>
+      <c r="C48" t="s">
         <v>59</v>
       </c>
-      <c r="C48" t="s">
-        <v>116</v>
-      </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2">
+        <v>45724</v>
+      </c>
+      <c r="C49" t="s">
         <v>60</v>
       </c>
-      <c r="C49" t="s">
-        <v>117</v>
-      </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="E49" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2">
+        <v>45725</v>
+      </c>
+      <c r="C50" t="s">
         <v>61</v>
       </c>
-      <c r="C50" t="s">
-        <v>118</v>
-      </c>
       <c r="D50" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2">
+        <v>45726</v>
+      </c>
+      <c r="C51" t="s">
         <v>62</v>
       </c>
-      <c r="C51" t="s">
-        <v>119</v>
-      </c>
       <c r="D51" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="E51" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2">
+        <v>45727</v>
+      </c>
+      <c r="C52" t="s">
         <v>63</v>
       </c>
-      <c r="C52" t="s">
-        <v>120</v>
-      </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2">
+        <v>45728</v>
+      </c>
+      <c r="C53" t="s">
         <v>64</v>
       </c>
-      <c r="C53" t="s">
-        <v>121</v>
-      </c>
       <c r="D53" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2">
+        <v>45729</v>
+      </c>
+      <c r="C54" t="s">
         <v>65</v>
       </c>
-      <c r="C54" t="s">
-        <v>122</v>
-      </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="E54" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2">
+        <v>45730</v>
+      </c>
+      <c r="C55" t="s">
         <v>66</v>
       </c>
-      <c r="C55" t="s">
-        <v>123</v>
-      </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2">
+        <v>45731</v>
+      </c>
+      <c r="C56" t="s">
         <v>67</v>
       </c>
-      <c r="C56" t="s">
-        <v>124</v>
-      </c>
       <c r="D56" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="E56" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2">
+        <v>45746</v>
+      </c>
+      <c r="C57" t="s">
         <v>68</v>
       </c>
-      <c r="C57" t="s">
-        <v>125</v>
-      </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2">
+        <v>45747</v>
+      </c>
+      <c r="C58" t="s">
         <v>69</v>
       </c>
-      <c r="C58" t="s">
-        <v>126</v>
-      </c>
       <c r="D58" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="E58" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E58">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented save survey and continue from past progress, prevent completed users from taking survey again
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B589EF58-73D3-4222-A332-11E6D91D5C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A90C81-019B-4D6F-9078-136072788C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="132">
   <si>
     <t>Week</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>I don’t want to show individual respondent scores</t>
+  </si>
+  <si>
+    <t>Add stop button to survey instances</t>
   </si>
 </sst>
 </file>
@@ -478,28 +484,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -807,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +806,7 @@
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +826,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -861,7 +846,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -881,7 +866,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -895,10 +880,13 @@
         <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -912,10 +900,16 @@
         <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45678</v>
+      </c>
+      <c r="G5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -929,10 +923,13 @@
         <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -946,10 +943,13 @@
         <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -963,10 +963,13 @@
         <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -983,120 +986,115 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2">
-        <v>45685</v>
-      </c>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>45686</v>
+        <v>45685</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>45687</v>
+        <v>45686</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2">
-        <v>45688</v>
+        <v>45687</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>45689</v>
+        <v>45688</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2">
+        <v>45689</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
         <v>45690</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>82</v>
-      </c>
-      <c r="E15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2">
-        <v>45691</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
       </c>
       <c r="E16" t="s">
         <v>126</v>
@@ -1107,13 +1105,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="2">
-        <v>45692</v>
+        <v>45691</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
         <v>126</v>
@@ -1124,13 +1122,13 @@
         <v>7</v>
       </c>
       <c r="B18" s="2">
-        <v>45693</v>
+        <v>45692</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
         <v>126</v>
@@ -1141,13 +1139,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="2">
-        <v>45694</v>
+        <v>45693</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
         <v>126</v>
@@ -1158,13 +1156,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="2">
-        <v>45695</v>
+        <v>45694</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
         <v>126</v>
@@ -1175,13 +1173,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="2">
-        <v>45696</v>
+        <v>45695</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
         <v>126</v>
@@ -1192,13 +1190,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="2">
-        <v>45697</v>
+        <v>45696</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>126</v>
@@ -1206,16 +1204,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>45698</v>
+        <v>45697</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
         <v>126</v>
@@ -1226,13 +1224,13 @@
         <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>45699</v>
+        <v>45698</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
         <v>126</v>
@@ -1243,13 +1241,13 @@
         <v>8</v>
       </c>
       <c r="B25" s="2">
-        <v>45700</v>
+        <v>45699</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
         <v>126</v>
@@ -1260,13 +1258,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="2">
-        <v>45701</v>
+        <v>45700</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
         <v>126</v>
@@ -1277,13 +1275,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="2">
-        <v>45702</v>
+        <v>45701</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
         <v>126</v>
@@ -1294,13 +1292,13 @@
         <v>8</v>
       </c>
       <c r="B28" s="2">
-        <v>45703</v>
+        <v>45702</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
         <v>126</v>
@@ -1311,13 +1309,13 @@
         <v>8</v>
       </c>
       <c r="B29" s="2">
-        <v>45704</v>
+        <v>45703</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
         <v>126</v>
@@ -1325,16 +1323,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="2">
-        <v>45705</v>
+        <v>45704</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
         <v>126</v>
@@ -1345,13 +1343,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>45706</v>
+        <v>45705</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
         <v>126</v>
@@ -1362,13 +1360,13 @@
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>45707</v>
+        <v>45706</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
         <v>126</v>
@@ -1379,13 +1377,13 @@
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>45708</v>
+        <v>45707</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
         <v>126</v>
@@ -1396,13 +1394,13 @@
         <v>9</v>
       </c>
       <c r="B34" s="2">
-        <v>45709</v>
+        <v>45708</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" t="s">
         <v>126</v>
@@ -1413,13 +1411,13 @@
         <v>9</v>
       </c>
       <c r="B35" s="2">
-        <v>45710</v>
+        <v>45709</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
         <v>126</v>
@@ -1430,13 +1428,13 @@
         <v>9</v>
       </c>
       <c r="B36" s="2">
-        <v>45711</v>
+        <v>45710</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
         <v>126</v>
@@ -1444,16 +1442,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2">
-        <v>45712</v>
+        <v>45711</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
         <v>126</v>
@@ -1464,13 +1462,13 @@
         <v>10</v>
       </c>
       <c r="B38" s="2">
-        <v>45713</v>
+        <v>45712</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E38" t="s">
         <v>126</v>
@@ -1481,13 +1479,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="2">
-        <v>45714</v>
+        <v>45713</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E39" t="s">
         <v>126</v>
@@ -1498,13 +1496,13 @@
         <v>10</v>
       </c>
       <c r="B40" s="2">
-        <v>45715</v>
+        <v>45714</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" t="s">
         <v>126</v>
@@ -1515,13 +1513,13 @@
         <v>10</v>
       </c>
       <c r="B41" s="2">
-        <v>45716</v>
+        <v>45715</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
         <v>126</v>
@@ -1532,13 +1530,13 @@
         <v>10</v>
       </c>
       <c r="B42" s="2">
-        <v>45717</v>
+        <v>45716</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E42" t="s">
         <v>126</v>
@@ -1549,13 +1547,13 @@
         <v>10</v>
       </c>
       <c r="B43" s="2">
-        <v>45718</v>
+        <v>45717</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
         <v>126</v>
@@ -1563,16 +1561,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="2">
-        <v>45719</v>
+        <v>45718</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E44" t="s">
         <v>126</v>
@@ -1583,13 +1581,13 @@
         <v>11</v>
       </c>
       <c r="B45" s="2">
-        <v>45720</v>
+        <v>45719</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" t="s">
         <v>126</v>
@@ -1600,13 +1598,13 @@
         <v>11</v>
       </c>
       <c r="B46" s="2">
-        <v>45721</v>
+        <v>45720</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" t="s">
         <v>126</v>
@@ -1617,13 +1615,13 @@
         <v>11</v>
       </c>
       <c r="B47" s="2">
-        <v>45722</v>
+        <v>45721</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
         <v>126</v>
@@ -1634,13 +1632,13 @@
         <v>11</v>
       </c>
       <c r="B48" s="2">
-        <v>45723</v>
+        <v>45722</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" t="s">
         <v>126</v>
@@ -1651,13 +1649,13 @@
         <v>11</v>
       </c>
       <c r="B49" s="2">
-        <v>45724</v>
+        <v>45723</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
         <v>126</v>
@@ -1668,13 +1666,13 @@
         <v>11</v>
       </c>
       <c r="B50" s="2">
-        <v>45725</v>
+        <v>45724</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E50" t="s">
         <v>126</v>
@@ -1685,13 +1683,13 @@
         <v>11</v>
       </c>
       <c r="B51" s="2">
-        <v>45726</v>
+        <v>45725</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E51" t="s">
         <v>126</v>
@@ -1702,13 +1700,13 @@
         <v>11</v>
       </c>
       <c r="B52" s="2">
-        <v>45727</v>
+        <v>45726</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E52" t="s">
         <v>126</v>
@@ -1719,13 +1717,13 @@
         <v>11</v>
       </c>
       <c r="B53" s="2">
-        <v>45728</v>
+        <v>45727</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E53" t="s">
         <v>126</v>
@@ -1736,13 +1734,13 @@
         <v>11</v>
       </c>
       <c r="B54" s="2">
-        <v>45729</v>
+        <v>45728</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E54" t="s">
         <v>126</v>
@@ -1753,13 +1751,13 @@
         <v>11</v>
       </c>
       <c r="B55" s="2">
-        <v>45730</v>
+        <v>45729</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
         <v>126</v>
@@ -1770,13 +1768,13 @@
         <v>11</v>
       </c>
       <c r="B56" s="2">
-        <v>45731</v>
+        <v>45730</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
         <v>126</v>
@@ -1784,16 +1782,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="2">
-        <v>45746</v>
+        <v>45731</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
         <v>126</v>
@@ -1804,21 +1802,38 @@
         <v>12</v>
       </c>
       <c r="B58" s="2">
+        <v>45746</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="2">
         <v>45747</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>69</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>125</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="E2:E59 G5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added edit and delete survey instance
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A90C81-019B-4D6F-9078-136072788C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F21309-C9E2-4659-B329-83364516E714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
   <si>
     <t>Week</t>
   </si>
@@ -415,7 +428,16 @@
     <t>I don’t want to show individual respondent scores</t>
   </si>
   <si>
-    <t>Add stop button to survey instances</t>
+    <t>Shows a message</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Edit survey instance details</t>
+  </si>
+  <si>
+    <t>Edit Survey</t>
   </si>
 </sst>
 </file>
@@ -447,7 +469,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -470,16 +492,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,10 +829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +844,7 @@
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,8 +863,15 @@
       <c r="F1" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="3">
+        <f>COUNTIF(E2:E59,"Done")/(COUNTIF(E2:E59,"Done")+COUNTIF(E2:E59,"Pending"))</f>
+        <v>0.25862068965517243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -846,7 +891,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -866,7 +911,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -886,7 +931,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -909,7 +954,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -929,7 +974,7 @@
         <v>45678</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -949,7 +994,7 @@
         <v>45678</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -969,7 +1014,7 @@
         <v>45678</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -983,90 +1028,116 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45685</v>
+      </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>45685</v>
+        <v>45686</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F11" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>45686</v>
+        <v>45687</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F12" s="2">
+        <v>45679</v>
+      </c>
+      <c r="G12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2">
-        <v>45687</v>
+        <v>45688</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>45688</v>
+        <v>45689</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F14" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1074,16 +1145,19 @@
         <v>45689</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F15" s="2">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1171,10 @@
         <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>129</v>
+      </c>
+      <c r="F16" s="2">
+        <v>45679</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added admin panel - survey instances
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F21309-C9E2-4659-B329-83364516E714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2ACB0C-4010-4886-9CCB-93D5E4A47F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="136">
   <si>
     <t>Week</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Edit Survey</t>
+  </si>
+  <si>
+    <t>Not planning for MVP</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +871,7 @@
       </c>
       <c r="H1" s="3">
         <f>COUNTIF(E2:E59,"Done")/(COUNTIF(E2:E59,"Done")+COUNTIF(E2:E59,"Pending"))</f>
-        <v>0.25862068965517243</v>
+        <v>0.29310344827586204</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1177,7 +1180,7 @@
         <v>45679</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1208,10 +1211,13 @@
         <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F18" s="2">
+        <v>45681</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1285,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1312,8 +1318,11 @@
       <c r="E24" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1329,8 +1338,11 @@
       <c r="E25" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1378,10 +1390,10 @@
         <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1398,7 +1410,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1415,7 +1427,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1432,7 +1444,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Added feature for summarizing text responses using chatgpt
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74979181-CC5A-4122-813D-AE99C7795FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB46CA5-E25B-47BA-908B-77CA0EC3B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
   <si>
     <t>Week</t>
   </si>
@@ -444,6 +447,9 @@
   </si>
   <si>
     <t>Not planned</t>
+  </si>
+  <si>
+    <t>New Completion Date</t>
   </si>
 </sst>
 </file>
@@ -546,6 +552,810 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Task</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Task Details</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Status</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Completed Date</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>Planned Completion Date</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Upload Survey Questions</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>Upload all existing survey questions into the system</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F2">
+            <v>45693</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Improve Survey Analytics UI</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Show category-wise and individual respondent scores</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F3">
+            <v>45694</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Progress Tracking in Survey</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Show question numbers while taking survey</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F4">
+            <v>45695</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Start Survey Saving Feature</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>Allow respondents to save incomplete surveys</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F5">
+            <v>45698</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Ensure Survey Resume Feature</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>Store saved responses and allow resumption</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F6">
+            <v>45699</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Survey Instance Validity</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>Add expiration dates to survey instances</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F7">
+            <v>45700</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Enforce Survey Expiry</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>Prevent submissions after survey validity ends</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F8">
+            <v>45701</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Stop Accepting Responses</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>Allow admins to manually stop survey responses</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F9">
+            <v>45702</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Hide Survey Form</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>Ensure UI hides form after stopping responses</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F10">
+            <v>45705</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Control Score Visibility</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>Hide scores until survey instance is closed</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F11">
+            <v>45706</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>Test Email Reminders</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>Ensure reminders work before survey expiry</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F12">
+            <v>45707</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Final Testing &amp; Bug Fixes</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>Test and fix new feature issues</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F13">
+            <v>45708</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Implement Survey Dashboard</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>Admin dashboard with survey statuses and engagement</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F14">
+            <v>45709</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Survey Engagement Metrics</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>Show survey instance completion rates</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F15">
+            <v>45712</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Enable CSV Export</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>Allow admins to export survey results</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F16">
+            <v>45713</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Optimize DB Queries</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>Improve survey data retrieval speed</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F17">
+            <v>45714</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>Improve UI Styling</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>Enhance user experience and layout</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F18">
+            <v>45715</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>System-Wide Security Test</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>Ensure access controls are correct</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F19">
+            <v>45716</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Clone Survey Feature</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>Allow users to duplicate surveys easily</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F20">
+            <v>45693</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Bulk Question Editing</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>Enable batch editing for survey questions</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F21">
+            <v>45694</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Allow Editing of Surveys</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>Enable admins to edit survey questions</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F22">
+            <v>45695</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Basic AI Insights</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>Suggest improvements based on survey scores</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F23">
+            <v>45698</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Improve AI Suggestions</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>Fine-tune survey recommendations</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F24">
+            <v>45699</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Email Notifications for Incomplete Surveys</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>Send reminders for unfinished surveys</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F25">
+            <v>45700</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Add Text Area Questions</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>Allow text-based responses in surveys</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F26">
+            <v>45701</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Implement Text Analysis</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>Analyze text responses for patterns</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F27">
+            <v>45702</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Optimize Mobile UI</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>Ensure smooth survey experience on mobile</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F28">
+            <v>45705</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>Mobile Performance Testing</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v>Check responsiveness on different devices</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F29">
+            <v>45706</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>Security Audit</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>Ensure no unauthorized data access</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F30">
+            <v>45707</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>Survey Performance Analytics</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>Track time taken per question</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F31">
+            <v>45708</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>Final UI Enhancements</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>Fix layout and responsiveness issues</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F32">
+            <v>45709</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>Test Large Surveys</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>Check system stability with large surveys</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F33">
+            <v>45712</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Fix Major Bugs</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>Resolve issues found during testing</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F34">
+            <v>45713</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Ensure Proper Survey Indexing</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>Optimize MongoDB indexes for faster queries</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F35">
+            <v>45714</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>Industry &amp; Category Filtering</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>Allow analytics based on industry selection</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F36">
+            <v>45715</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>Optimize Email System</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>Ensure bulk emails don’t get marked as spam</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F37">
+            <v>45716</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Final Survey Completion Reminders</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>Last-minute reminders to respondents</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F38">
+            <v>45693</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Final Bug Fixes</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>Resolve remaining issues before feature freeze</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F39">
+            <v>45694</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>Feature Freeze</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>Lock features and start final testing</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F40">
+            <v>45695</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Final Pre-March Testing</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>Ensure everything works smoothly</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F41">
+            <v>45698</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>Full System Testing</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>Check all workflows for stability</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F42">
+            <v>45699</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>Implement Extra Security Measures</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>Enhance access controls</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F43">
+            <v>45700</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v>Final Review of Survey Workflows</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>Ensure smooth user journey</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F44">
+            <v>45701</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45" t="str">
+            <v>Multi-User Testing</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>Check for performance issues with concurrent users</v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F45">
+            <v>45702</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46" t="str">
+            <v>Fix Load Testing Issues</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>Resolve any problems found</v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F46">
+            <v>45705</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47" t="str">
+            <v>Prepare for Beta Testing</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>Identify users for testing</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F47">
+            <v>45706</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48" t="str">
+            <v>Feedback Collection Mechanism</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>Allow users to leave feedback on surveys</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F48">
+            <v>45707</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49" t="str">
+            <v>Final Mobile Optimization</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v>Ensure surveys work flawlessly on mobile</v>
+          </cell>
+          <cell r="D49" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F49">
+            <v>45708</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50" t="str">
+            <v>Stress Testing</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>Test system under heavy load</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F50">
+            <v>45709</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51" t="str">
+            <v>Security Patches</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>Implement final security improvements</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F51">
+            <v>45712</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52" t="str">
+            <v>Final System Test Before Break</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>Ensure everything is ready</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F52">
+            <v>45713</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53" t="str">
+            <v>Documentation</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v>Write internal documentation for admins</v>
+          </cell>
+          <cell r="D53" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F53">
+            <v>45714</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54" t="str">
+            <v>Final Bug Fixes &amp; Feature Lock</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>Fix last-minute issues</v>
+          </cell>
+          <cell r="D54" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F54">
+            <v>45715</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="B55" t="str">
+            <v>Post-Break System Review</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>Check for any unexpected issues</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F55">
+            <v>45716</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="B56" t="str">
+            <v>Final Launch &amp; Internal Rollout</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v>Deploy system for usage</v>
+          </cell>
+          <cell r="D56" t="str">
+            <v>Pending</v>
+          </cell>
+          <cell r="F56">
+            <v>45693</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -835,11 +1645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,9 +1658,10 @@
     <col min="4" max="4" width="64.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,14 +1681,17 @@
         <v>127</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="3">
+      <c r="I1" s="3">
         <f>COUNTIF(E2:E59,"Done")/(COUNTIF(E2:E59,"Done")+COUNTIF(E2:E59,"Pending"))</f>
         <v>0.32142857142857145</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -896,8 +1710,12 @@
       <c r="F2" s="2">
         <v>45677</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="str">
+        <f>IF(E2="Done","",IF(E2="Not planned","",VLOOKUP(C2,[1]Sheet1!$B:$F,5,0)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -916,8 +1734,12 @@
       <c r="F3" s="2">
         <v>45677</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="str">
+        <f>IF(E3="Done","",IF(E3="Not planned","",VLOOKUP(C3,[1]Sheet1!$B:$F,5,0)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -936,8 +1758,12 @@
       <c r="F4" s="2">
         <v>45677</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="str">
+        <f>IF(E4="Done","",IF(E4="Not planned","",VLOOKUP(C4,[1]Sheet1!$B:$F,5,0)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -956,11 +1782,15 @@
       <c r="F5" s="2">
         <v>45678</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="str">
+        <f>IF(E5="Done","",IF(E5="Not planned","",VLOOKUP(C5,[1]Sheet1!$B:$F,5,0)))</f>
+        <v/>
+      </c>
+      <c r="H5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -979,8 +1809,12 @@
       <c r="F6" s="2">
         <v>45678</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="str">
+        <f>IF(E6="Done","",IF(E6="Not planned","",VLOOKUP(C6,[1]Sheet1!$B:$F,5,0)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -999,8 +1833,9 @@
       <c r="F7" s="2">
         <v>45678</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1019,8 +1854,9 @@
       <c r="F8" s="2">
         <v>45678</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1039,8 +1875,9 @@
       <c r="F9" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1059,8 +1896,9 @@
       <c r="F10" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1079,8 +1917,9 @@
       <c r="F11" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1099,11 +1938,12 @@
       <c r="F12" s="2">
         <v>45679</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1122,8 +1962,9 @@
       <c r="F13" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1142,8 +1983,9 @@
       <c r="F14" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1162,8 +2004,9 @@
       <c r="F15" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1182,8 +2025,9 @@
       <c r="F16" s="2">
         <v>45679</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1199,8 +2043,9 @@
       <c r="E17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1219,8 +2064,9 @@
       <c r="F18" s="2">
         <v>45681</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1236,8 +2082,11 @@
       <c r="E19" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="2">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1253,8 +2102,11 @@
       <c r="E20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="2">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +2122,11 @@
       <c r="E21" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="2">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1287,8 +2142,11 @@
       <c r="E22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="2">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1304,8 +2162,12 @@
       <c r="E23" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+      <c r="H23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1321,11 +2183,12 @@
       <c r="E24" t="s">
         <v>136</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1341,11 +2204,11 @@
       <c r="E25" t="s">
         <v>136</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1361,8 +2224,11 @@
       <c r="E26" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="2">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1378,8 +2244,11 @@
       <c r="E27" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="2">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1395,8 +2264,9 @@
       <c r="E28" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1412,8 +2282,9 @@
       <c r="E29" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1429,8 +2300,11 @@
       <c r="E30" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="2">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1446,8 +2320,11 @@
       <c r="E31" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="2">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1463,8 +2340,11 @@
       <c r="E32" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="2">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1480,8 +2360,11 @@
       <c r="E33" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" s="2">
+        <v>45696</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1497,8 +2380,9 @@
       <c r="E34" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1514,8 +2398,9 @@
       <c r="E35" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1531,8 +2416,9 @@
       <c r="E36" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1548,8 +2434,9 @@
       <c r="E37" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1565,8 +2452,9 @@
       <c r="E38" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1582,8 +2470,9 @@
       <c r="E39" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1599,8 +2488,9 @@
       <c r="E40" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1616,8 +2506,9 @@
       <c r="E41" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1633,8 +2524,9 @@
       <c r="E42" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1650,8 +2542,9 @@
       <c r="E43" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1667,8 +2560,9 @@
       <c r="E44" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -1684,8 +2578,9 @@
       <c r="E45" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -1701,8 +2596,9 @@
       <c r="E46" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1718,8 +2614,9 @@
       <c r="E47" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -1735,8 +2632,9 @@
       <c r="E48" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1752,8 +2650,9 @@
       <c r="E49" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -1769,8 +2668,9 @@
       <c r="E50" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1786,8 +2686,9 @@
       <c r="E51" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -1803,8 +2704,9 @@
       <c r="E52" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -1820,8 +2722,9 @@
       <c r="E53" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1837,8 +2740,9 @@
       <c r="E54" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -1854,8 +2758,9 @@
       <c r="E55" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1871,8 +2776,9 @@
       <c r="E56" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -1888,8 +2794,9 @@
       <c r="E57" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -1905,8 +2812,9 @@
       <c r="E58" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -1922,9 +2830,10 @@
       <c r="E59" t="s">
         <v>126</v>
       </c>
+      <c r="G59" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E59 G5">
+  <conditionalFormatting sqref="E2:E59 H5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Modified survey home page
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\pricePelican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB46CA5-E25B-47BA-908B-77CA0EC3B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F258F6-022C-427D-9F90-82F5B16A9496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="137">
   <si>
     <t>Week</t>
   </si>
@@ -447,9 +444,6 @@
   </si>
   <si>
     <t>Not planned</t>
-  </si>
-  <si>
-    <t>New Completion Date</t>
   </si>
 </sst>
 </file>
@@ -552,810 +546,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Task</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Task Details</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Status</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Completed Date</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>Planned Completion Date</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Upload Survey Questions</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Upload all existing survey questions into the system</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F2">
-            <v>45693</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Improve Survey Analytics UI</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>Show category-wise and individual respondent scores</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F3">
-            <v>45694</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Progress Tracking in Survey</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>Show question numbers while taking survey</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F4">
-            <v>45695</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Start Survey Saving Feature</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>Allow respondents to save incomplete surveys</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F5">
-            <v>45698</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Ensure Survey Resume Feature</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>Store saved responses and allow resumption</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F6">
-            <v>45699</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Survey Instance Validity</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>Add expiration dates to survey instances</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F7">
-            <v>45700</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Enforce Survey Expiry</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>Prevent submissions after survey validity ends</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F8">
-            <v>45701</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Stop Accepting Responses</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>Allow admins to manually stop survey responses</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F9">
-            <v>45702</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Hide Survey Form</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>Ensure UI hides form after stopping responses</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F10">
-            <v>45705</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Control Score Visibility</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>Hide scores until survey instance is closed</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F11">
-            <v>45706</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>Test Email Reminders</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>Ensure reminders work before survey expiry</v>
-          </cell>
-          <cell r="D12" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F12">
-            <v>45707</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Final Testing &amp; Bug Fixes</v>
-          </cell>
-          <cell r="C13" t="str">
-            <v>Test and fix new feature issues</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F13">
-            <v>45708</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Implement Survey Dashboard</v>
-          </cell>
-          <cell r="C14" t="str">
-            <v>Admin dashboard with survey statuses and engagement</v>
-          </cell>
-          <cell r="D14" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F14">
-            <v>45709</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>Survey Engagement Metrics</v>
-          </cell>
-          <cell r="C15" t="str">
-            <v>Show survey instance completion rates</v>
-          </cell>
-          <cell r="D15" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F15">
-            <v>45712</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Enable CSV Export</v>
-          </cell>
-          <cell r="C16" t="str">
-            <v>Allow admins to export survey results</v>
-          </cell>
-          <cell r="D16" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F16">
-            <v>45713</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Optimize DB Queries</v>
-          </cell>
-          <cell r="C17" t="str">
-            <v>Improve survey data retrieval speed</v>
-          </cell>
-          <cell r="D17" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F17">
-            <v>45714</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>Improve UI Styling</v>
-          </cell>
-          <cell r="C18" t="str">
-            <v>Enhance user experience and layout</v>
-          </cell>
-          <cell r="D18" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F18">
-            <v>45715</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>System-Wide Security Test</v>
-          </cell>
-          <cell r="C19" t="str">
-            <v>Ensure access controls are correct</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F19">
-            <v>45716</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>Clone Survey Feature</v>
-          </cell>
-          <cell r="C20" t="str">
-            <v>Allow users to duplicate surveys easily</v>
-          </cell>
-          <cell r="D20" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F20">
-            <v>45693</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>Bulk Question Editing</v>
-          </cell>
-          <cell r="C21" t="str">
-            <v>Enable batch editing for survey questions</v>
-          </cell>
-          <cell r="D21" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F21">
-            <v>45694</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Allow Editing of Surveys</v>
-          </cell>
-          <cell r="C22" t="str">
-            <v>Enable admins to edit survey questions</v>
-          </cell>
-          <cell r="D22" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F22">
-            <v>45695</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Basic AI Insights</v>
-          </cell>
-          <cell r="C23" t="str">
-            <v>Suggest improvements based on survey scores</v>
-          </cell>
-          <cell r="D23" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F23">
-            <v>45698</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v>Improve AI Suggestions</v>
-          </cell>
-          <cell r="C24" t="str">
-            <v>Fine-tune survey recommendations</v>
-          </cell>
-          <cell r="D24" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F24">
-            <v>45699</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>Email Notifications for Incomplete Surveys</v>
-          </cell>
-          <cell r="C25" t="str">
-            <v>Send reminders for unfinished surveys</v>
-          </cell>
-          <cell r="D25" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F25">
-            <v>45700</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Add Text Area Questions</v>
-          </cell>
-          <cell r="C26" t="str">
-            <v>Allow text-based responses in surveys</v>
-          </cell>
-          <cell r="D26" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F26">
-            <v>45701</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Implement Text Analysis</v>
-          </cell>
-          <cell r="C27" t="str">
-            <v>Analyze text responses for patterns</v>
-          </cell>
-          <cell r="D27" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F27">
-            <v>45702</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Optimize Mobile UI</v>
-          </cell>
-          <cell r="C28" t="str">
-            <v>Ensure smooth survey experience on mobile</v>
-          </cell>
-          <cell r="D28" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F28">
-            <v>45705</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v>Mobile Performance Testing</v>
-          </cell>
-          <cell r="C29" t="str">
-            <v>Check responsiveness on different devices</v>
-          </cell>
-          <cell r="D29" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F29">
-            <v>45706</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Security Audit</v>
-          </cell>
-          <cell r="C30" t="str">
-            <v>Ensure no unauthorized data access</v>
-          </cell>
-          <cell r="D30" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F30">
-            <v>45707</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>Survey Performance Analytics</v>
-          </cell>
-          <cell r="C31" t="str">
-            <v>Track time taken per question</v>
-          </cell>
-          <cell r="D31" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F31">
-            <v>45708</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Final UI Enhancements</v>
-          </cell>
-          <cell r="C32" t="str">
-            <v>Fix layout and responsiveness issues</v>
-          </cell>
-          <cell r="D32" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F32">
-            <v>45709</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>Test Large Surveys</v>
-          </cell>
-          <cell r="C33" t="str">
-            <v>Check system stability with large surveys</v>
-          </cell>
-          <cell r="D33" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F33">
-            <v>45712</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Fix Major Bugs</v>
-          </cell>
-          <cell r="C34" t="str">
-            <v>Resolve issues found during testing</v>
-          </cell>
-          <cell r="D34" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F34">
-            <v>45713</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>Ensure Proper Survey Indexing</v>
-          </cell>
-          <cell r="C35" t="str">
-            <v>Optimize MongoDB indexes for faster queries</v>
-          </cell>
-          <cell r="D35" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F35">
-            <v>45714</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v>Industry &amp; Category Filtering</v>
-          </cell>
-          <cell r="C36" t="str">
-            <v>Allow analytics based on industry selection</v>
-          </cell>
-          <cell r="D36" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F36">
-            <v>45715</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>Optimize Email System</v>
-          </cell>
-          <cell r="C37" t="str">
-            <v>Ensure bulk emails don’t get marked as spam</v>
-          </cell>
-          <cell r="D37" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F37">
-            <v>45716</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>Final Survey Completion Reminders</v>
-          </cell>
-          <cell r="C38" t="str">
-            <v>Last-minute reminders to respondents</v>
-          </cell>
-          <cell r="D38" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F38">
-            <v>45693</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Final Bug Fixes</v>
-          </cell>
-          <cell r="C39" t="str">
-            <v>Resolve remaining issues before feature freeze</v>
-          </cell>
-          <cell r="D39" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F39">
-            <v>45694</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>Feature Freeze</v>
-          </cell>
-          <cell r="C40" t="str">
-            <v>Lock features and start final testing</v>
-          </cell>
-          <cell r="D40" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F40">
-            <v>45695</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Final Pre-March Testing</v>
-          </cell>
-          <cell r="C41" t="str">
-            <v>Ensure everything works smoothly</v>
-          </cell>
-          <cell r="D41" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F41">
-            <v>45698</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>Full System Testing</v>
-          </cell>
-          <cell r="C42" t="str">
-            <v>Check all workflows for stability</v>
-          </cell>
-          <cell r="D42" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F42">
-            <v>45699</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v>Implement Extra Security Measures</v>
-          </cell>
-          <cell r="C43" t="str">
-            <v>Enhance access controls</v>
-          </cell>
-          <cell r="D43" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F43">
-            <v>45700</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44" t="str">
-            <v>Final Review of Survey Workflows</v>
-          </cell>
-          <cell r="C44" t="str">
-            <v>Ensure smooth user journey</v>
-          </cell>
-          <cell r="D44" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F44">
-            <v>45701</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45" t="str">
-            <v>Multi-User Testing</v>
-          </cell>
-          <cell r="C45" t="str">
-            <v>Check for performance issues with concurrent users</v>
-          </cell>
-          <cell r="D45" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F45">
-            <v>45702</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>Fix Load Testing Issues</v>
-          </cell>
-          <cell r="C46" t="str">
-            <v>Resolve any problems found</v>
-          </cell>
-          <cell r="D46" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F46">
-            <v>45705</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47" t="str">
-            <v>Prepare for Beta Testing</v>
-          </cell>
-          <cell r="C47" t="str">
-            <v>Identify users for testing</v>
-          </cell>
-          <cell r="D47" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F47">
-            <v>45706</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48" t="str">
-            <v>Feedback Collection Mechanism</v>
-          </cell>
-          <cell r="C48" t="str">
-            <v>Allow users to leave feedback on surveys</v>
-          </cell>
-          <cell r="D48" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F48">
-            <v>45707</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49" t="str">
-            <v>Final Mobile Optimization</v>
-          </cell>
-          <cell r="C49" t="str">
-            <v>Ensure surveys work flawlessly on mobile</v>
-          </cell>
-          <cell r="D49" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F49">
-            <v>45708</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>Stress Testing</v>
-          </cell>
-          <cell r="C50" t="str">
-            <v>Test system under heavy load</v>
-          </cell>
-          <cell r="D50" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F50">
-            <v>45709</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51" t="str">
-            <v>Security Patches</v>
-          </cell>
-          <cell r="C51" t="str">
-            <v>Implement final security improvements</v>
-          </cell>
-          <cell r="D51" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F51">
-            <v>45712</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52" t="str">
-            <v>Final System Test Before Break</v>
-          </cell>
-          <cell r="C52" t="str">
-            <v>Ensure everything is ready</v>
-          </cell>
-          <cell r="D52" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F52">
-            <v>45713</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53" t="str">
-            <v>Documentation</v>
-          </cell>
-          <cell r="C53" t="str">
-            <v>Write internal documentation for admins</v>
-          </cell>
-          <cell r="D53" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F53">
-            <v>45714</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54" t="str">
-            <v>Final Bug Fixes &amp; Feature Lock</v>
-          </cell>
-          <cell r="C54" t="str">
-            <v>Fix last-minute issues</v>
-          </cell>
-          <cell r="D54" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F54">
-            <v>45715</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55" t="str">
-            <v>Post-Break System Review</v>
-          </cell>
-          <cell r="C55" t="str">
-            <v>Check for any unexpected issues</v>
-          </cell>
-          <cell r="D55" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F55">
-            <v>45716</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56" t="str">
-            <v>Final Launch &amp; Internal Rollout</v>
-          </cell>
-          <cell r="C56" t="str">
-            <v>Deploy system for usage</v>
-          </cell>
-          <cell r="D56" t="str">
-            <v>Pending</v>
-          </cell>
-          <cell r="F56">
-            <v>45693</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1645,11 +835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,10 +848,9 @@
     <col min="4" max="4" width="64.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,17 +870,14 @@
         <v>127</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="3">
+      <c r="H1" s="3">
         <f>COUNTIF(E2:E59,"Done")/(COUNTIF(E2:E59,"Done")+COUNTIF(E2:E59,"Pending"))</f>
-        <v>0.32142857142857145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3392857142857143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1710,12 +896,8 @@
       <c r="F2" s="2">
         <v>45677</v>
       </c>
-      <c r="G2" s="2" t="str">
-        <f>IF(E2="Done","",IF(E2="Not planned","",VLOOKUP(C2,[1]Sheet1!$B:$F,5,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1734,12 +916,8 @@
       <c r="F3" s="2">
         <v>45677</v>
       </c>
-      <c r="G3" s="2" t="str">
-        <f>IF(E3="Done","",IF(E3="Not planned","",VLOOKUP(C3,[1]Sheet1!$B:$F,5,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1758,12 +936,8 @@
       <c r="F4" s="2">
         <v>45677</v>
       </c>
-      <c r="G4" s="2" t="str">
-        <f>IF(E4="Done","",IF(E4="Not planned","",VLOOKUP(C4,[1]Sheet1!$B:$F,5,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1782,15 +956,11 @@
       <c r="F5" s="2">
         <v>45678</v>
       </c>
-      <c r="G5" s="2" t="str">
-        <f>IF(E5="Done","",IF(E5="Not planned","",VLOOKUP(C5,[1]Sheet1!$B:$F,5,0)))</f>
-        <v/>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1809,12 +979,8 @@
       <c r="F6" s="2">
         <v>45678</v>
       </c>
-      <c r="G6" s="2" t="str">
-        <f>IF(E6="Done","",IF(E6="Not planned","",VLOOKUP(C6,[1]Sheet1!$B:$F,5,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1833,9 +999,8 @@
       <c r="F7" s="2">
         <v>45678</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1854,9 +1019,8 @@
       <c r="F8" s="2">
         <v>45678</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1875,9 +1039,8 @@
       <c r="F9" s="2">
         <v>45679</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1896,9 +1059,8 @@
       <c r="F10" s="2">
         <v>45679</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1917,9 +1079,8 @@
       <c r="F11" s="2">
         <v>45679</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1938,12 +1099,11 @@
       <c r="F12" s="2">
         <v>45679</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1962,9 +1122,8 @@
       <c r="F13" s="2">
         <v>45679</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1983,9 +1142,8 @@
       <c r="F14" s="2">
         <v>45679</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2004,9 +1162,8 @@
       <c r="F15" s="2">
         <v>45679</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2025,9 +1182,8 @@
       <c r="F16" s="2">
         <v>45679</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2043,9 +1199,8 @@
       <c r="E17" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2064,9 +1219,8 @@
       <c r="F18" s="2">
         <v>45681</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2082,11 +1236,8 @@
       <c r="E19" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="2">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2102,11 +1253,8 @@
       <c r="E20" t="s">
         <v>126</v>
       </c>
-      <c r="G20" s="2">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2122,11 +1270,8 @@
       <c r="E21" t="s">
         <v>126</v>
       </c>
-      <c r="G21" s="2">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -2142,11 +1287,8 @@
       <c r="E22" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="2">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -2162,12 +1304,11 @@
       <c r="E23" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2183,12 +1324,11 @@
       <c r="E24" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2204,11 +1344,11 @@
       <c r="E25" t="s">
         <v>136</v>
       </c>
-      <c r="H25" t="s">
+      <c r="G25" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2224,11 +1364,8 @@
       <c r="E26" t="s">
         <v>126</v>
       </c>
-      <c r="G26" s="2">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2244,11 +1381,8 @@
       <c r="E27" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="2">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2264,9 +1398,8 @@
       <c r="E28" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2282,9 +1415,8 @@
       <c r="E29" t="s">
         <v>129</v>
       </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2298,13 +1430,13 @@
         <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" s="2">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F30" s="2">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2320,11 +1452,8 @@
       <c r="E31" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="2">
-        <v>45695</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2340,11 +1469,8 @@
       <c r="E32" t="s">
         <v>126</v>
       </c>
-      <c r="G32" s="2">
-        <v>45695</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2360,11 +1486,8 @@
       <c r="E33" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="2">
-        <v>45696</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2380,9 +1503,8 @@
       <c r="E34" t="s">
         <v>126</v>
       </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2398,9 +1520,8 @@
       <c r="E35" t="s">
         <v>126</v>
       </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2416,9 +1537,8 @@
       <c r="E36" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2434,9 +1554,8 @@
       <c r="E37" t="s">
         <v>126</v>
       </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2452,9 +1571,8 @@
       <c r="E38" t="s">
         <v>126</v>
       </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2470,9 +1588,8 @@
       <c r="E39" t="s">
         <v>126</v>
       </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2488,9 +1605,8 @@
       <c r="E40" t="s">
         <v>126</v>
       </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2506,9 +1622,8 @@
       <c r="E41" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2524,9 +1639,8 @@
       <c r="E42" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2542,9 +1656,8 @@
       <c r="E43" t="s">
         <v>126</v>
       </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2560,9 +1673,8 @@
       <c r="E44" t="s">
         <v>126</v>
       </c>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2578,9 +1690,8 @@
       <c r="E45" t="s">
         <v>126</v>
       </c>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2596,9 +1707,8 @@
       <c r="E46" t="s">
         <v>126</v>
       </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2614,9 +1724,8 @@
       <c r="E47" t="s">
         <v>126</v>
       </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2632,9 +1741,8 @@
       <c r="E48" t="s">
         <v>126</v>
       </c>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2650,9 +1758,8 @@
       <c r="E49" t="s">
         <v>126</v>
       </c>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2668,9 +1775,8 @@
       <c r="E50" t="s">
         <v>126</v>
       </c>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2686,9 +1792,8 @@
       <c r="E51" t="s">
         <v>126</v>
       </c>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -2704,9 +1809,8 @@
       <c r="E52" t="s">
         <v>126</v>
       </c>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2722,9 +1826,8 @@
       <c r="E53" t="s">
         <v>126</v>
       </c>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -2740,9 +1843,8 @@
       <c r="E54" t="s">
         <v>126</v>
       </c>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -2758,9 +1860,8 @@
       <c r="E55" t="s">
         <v>126</v>
       </c>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -2776,9 +1877,8 @@
       <c r="E56" t="s">
         <v>126</v>
       </c>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2794,9 +1894,8 @@
       <c r="E57" t="s">
         <v>126</v>
       </c>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2812,9 +1911,8 @@
       <c r="E58" t="s">
         <v>126</v>
       </c>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -2830,10 +1928,9 @@
       <c r="E59" t="s">
         <v>126</v>
       </c>
-      <c r="G59" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E59 H5">
+  <conditionalFormatting sqref="E2:E59 G5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>

</xml_diff>